<commit_message>
Em-dash to - in captions
</commit_message>
<xml_diff>
--- a/data/Milestones_COVID-19.xlsx
+++ b/data/Milestones_COVID-19.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Documents/covid_aggr_data_scripts_before_github_2022-03-08/preliminaryproj_covidpsychservices/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Documents/git/covid_psyserv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8460C990-90BF-7142-9A11-65713356FCF7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B4CB8C-D587-4042-ADD1-124B9F401BDB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7900" yWindow="1580" windowWidth="15400" windowHeight="14440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7900" yWindow="1580" windowWidth="15400" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="2" r:id="rId1"/>
@@ -33,24 +33,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Distance schooling for 16–19 year-olds, Helsinki region</t>
-  </si>
-  <si>
-    <t>Distance schooling for 13–19 year-olds, nationwide</t>
-  </si>
-  <si>
-    <t>Distance schooling for 13–19 year-olds, Helsinki and certain other regions</t>
-  </si>
-  <si>
     <t>label</t>
   </si>
   <si>
     <t>Lockdown of Helsinki University Hospital region</t>
   </si>
   <si>
-    <t>Distance schooling for 7–19 year-olds, nationwide</t>
-  </si>
-  <si>
     <t>height_rect</t>
   </si>
   <si>
@@ -75,7 +63,19 @@
     <t>ymin</t>
   </si>
   <si>
-    <t>Distance schooling for 13–19 year-olds in various regions</t>
+    <t>Distance schooling for 7-19 year-olds, nationwide</t>
+  </si>
+  <si>
+    <t>Distance schooling for 13-19 year-olds in various regions</t>
+  </si>
+  <si>
+    <t>Distance schooling for 16-19 year-olds, Helsinki region</t>
+  </si>
+  <si>
+    <t>Distance schooling for 13-19 year-olds, Helsinki and certain other regions</t>
+  </si>
+  <si>
+    <t>Distance schooling for 13-19 year-olds, nationwide</t>
   </si>
 </sst>
 </file>
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF107CA-CC4F-6641-97F6-19E7B01EE637}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -408,22 +408,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -445,7 +445,7 @@
         <v>43936</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -467,7 +467,7 @@
         <v>43965</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -489,7 +489,7 @@
         <v>44297</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -511,7 +511,7 @@
         <v>44284</v>
       </c>
       <c r="F5" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -533,7 +533,7 @@
         <v>44297</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -555,7 +555,7 @@
         <v>44283</v>
       </c>
       <c r="F7" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>-52</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -571,7 +571,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -579,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C661CBC5-CF7F-F943-8D0A-B4EBFF27272A}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -668,7 +668,7 @@
       </c>
       <c r="F3" t="str">
         <f>original!F3</f>
-        <v>Distance schooling for 7–19 year-olds, nationwide</v>
+        <v>Distance schooling for 7-19 year-olds, nationwide</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -692,7 +692,7 @@
       </c>
       <c r="F4" t="str">
         <f>original!F4</f>
-        <v>Distance schooling for 13–19 year-olds in various regions</v>
+        <v>Distance schooling for 13-19 year-olds in various regions</v>
       </c>
     </row>
   </sheetData>

</xml_diff>